<commit_message>
spreadsheet with data per municipality
</commit_message>
<xml_diff>
--- a/public/Spreadsheets/yearlyRevenueOverview.xlsx
+++ b/public/Spreadsheets/yearlyRevenueOverview.xlsx
@@ -15,7 +15,86 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+  <si>
+    <t>Total revenue</t>
+  </si>
+  <si>
+    <t>06-2022 - 07-2022</t>
+  </si>
+  <si>
+    <t>07-2022 - 08-2022</t>
+  </si>
+  <si>
+    <t>08-2022 - 09-2022</t>
+  </si>
+  <si>
+    <t>09-2022 - 10-2022</t>
+  </si>
+  <si>
+    <t>10-2022 - 11-2022</t>
+  </si>
+  <si>
+    <t>11-2022 - 12-2022</t>
+  </si>
+  <si>
+    <t>12-2022 - 01-2023</t>
+  </si>
+  <si>
+    <t>01-2023 - 02-2023</t>
+  </si>
+  <si>
+    <t>02-2023 - 03-2023</t>
+  </si>
+  <si>
+    <t>03-2023 - 04-2023</t>
+  </si>
+  <si>
+    <t>04-2023 - 05-2023</t>
+  </si>
+  <si>
+    <t>05-2023 - 06-2023</t>
+  </si>
+  <si>
+    <t>€12176.026</t>
+  </si>
+  <si>
+    <t>€643.72</t>
+  </si>
+  <si>
+    <t>€1070.82</t>
+  </si>
+  <si>
+    <t>€1089.03</t>
+  </si>
+  <si>
+    <t>€738.71</t>
+  </si>
+  <si>
+    <t>€1066.35</t>
+  </si>
+  <si>
+    <t>€862.51</t>
+  </si>
+  <si>
+    <t>€1468.42</t>
+  </si>
+  <si>
+    <t>€1442.73</t>
+  </si>
+  <si>
+    <t>€696.71</t>
+  </si>
+  <si>
+    <t>€1641.07</t>
+  </si>
+  <si>
+    <t>€955.64</t>
+  </si>
+  <si>
+    <t>€500.3</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -363,102 +442,109 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.569" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="11.711" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="11.711" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="10.569" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="10.569" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="10.569" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="11.711" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="11.711" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="10.569" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="11.711" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="10.569" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="10.569" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="21.138" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="1">
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2">
-        <v>643.7237</v>
-      </c>
-      <c r="B2">
-        <v>1070.8186</v>
-      </c>
-      <c r="C2">
-        <v>1089.0335</v>
-      </c>
-      <c r="D2">
-        <v>738.7094</v>
-      </c>
-      <c r="E2">
-        <v>1066.351</v>
-      </c>
-      <c r="F2">
-        <v>862.5107</v>
-      </c>
-      <c r="G2">
-        <v>1468.4219</v>
-      </c>
-      <c r="H2">
-        <v>1442.7321</v>
-      </c>
-      <c r="I2">
-        <v>696.7085</v>
-      </c>
-      <c r="J2">
-        <v>1641.0739</v>
-      </c>
-      <c r="K2">
-        <v>955.6382</v>
-      </c>
-      <c r="L2">
-        <v>500.3042</v>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing bug in customer sheet, make year&quarter
</commit_message>
<xml_diff>
--- a/public/Spreadsheets/yearlyRevenueOverview.xlsx
+++ b/public/Spreadsheets/yearlyRevenueOverview.xlsx
@@ -56,13 +56,13 @@
     <t>05-2023 - 06-2023</t>
   </si>
   <si>
-    <t>€12176.026</t>
-  </si>
-  <si>
-    <t>€643.72</t>
-  </si>
-  <si>
-    <t>€1070.82</t>
+    <t>€14162.725</t>
+  </si>
+  <si>
+    <t>€715.28</t>
+  </si>
+  <si>
+    <t>€1275.77</t>
   </si>
   <si>
     <t>€1089.03</t>
@@ -71,28 +71,28 @@
     <t>€738.71</t>
   </si>
   <si>
-    <t>€1066.35</t>
-  </si>
-  <si>
-    <t>€862.51</t>
-  </si>
-  <si>
-    <t>€1468.42</t>
-  </si>
-  <si>
-    <t>€1442.73</t>
-  </si>
-  <si>
-    <t>€696.71</t>
-  </si>
-  <si>
-    <t>€1641.07</t>
-  </si>
-  <si>
-    <t>€955.64</t>
-  </si>
-  <si>
-    <t>€500.3</t>
+    <t>€1227.9</t>
+  </si>
+  <si>
+    <t>€522.32</t>
+  </si>
+  <si>
+    <t>€1101.1</t>
+  </si>
+  <si>
+    <t>€1720.3</t>
+  </si>
+  <si>
+    <t>€1614.23</t>
+  </si>
+  <si>
+    <t>€1150.56</t>
+  </si>
+  <si>
+    <t>€1976.16</t>
+  </si>
+  <si>
+    <t>€1031.36</t>
   </si>
 </sst>
 </file>

</xml_diff>